<commit_message>
Added PT municipalities and parishes list of douro municipalities - working on map
</commit_message>
<xml_diff>
--- a/data_source/douro/douro_wine_producers_list.xlsx
+++ b/data_source/douro/douro_wine_producers_list.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GIS_Master\Semester2\EGM722\Assigment\wine_project\data_source\douro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8777F76C-05E7-4033-8E80-FC5D5348254D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E561623F-80A7-4CE5-B6EA-C1F807B29C89}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{3922B37A-1043-47D6-93D5-73929D5CD50D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$249</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,30 +37,198 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>Niepoort</t>
-  </si>
-  <si>
-    <t xml:space="preserve">670 Rua Candido do Reis, Vila Nova de Gaia 4400 </t>
-  </si>
-  <si>
-    <t>Poeira</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Provesende 5060, Villa Real </t>
-  </si>
-  <si>
-    <t>Quinta do Couquinho</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Horta da Vilarica, 5160-101 Torre de Moncorvo, Douro </t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+  <si>
+    <t>Quinta do Judeu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estrada EM313, Peso da Regua 5050, Vila Real </t>
+  </si>
+  <si>
+    <t>Adega Cooperativa de Mesao Frio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avenida Dr. Domingos Monteiro Fundo de Vila, 5040-909 Mesao Frio, Vila Real </t>
+  </si>
+  <si>
+    <t>Adega Cooperativa de Sabrosa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rua das Flores 27, Alto de Paços, 5060-321 Sabrosa, Vila Real </t>
+  </si>
+  <si>
+    <t>Adega Vila Real</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vale Frio - Folhadela, Vila Real 5000 </t>
+  </si>
+  <si>
+    <t>Aneto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quinta do Paco, 5050-090 Godim, Vila Real </t>
   </si>
   <si>
     <t>producer</t>
   </si>
   <si>
     <t>address</t>
+  </si>
+  <si>
+    <t>Bago de Touriga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Urb Vila Paulista, 5000-262 Vila Real, Douro </t>
+  </si>
+  <si>
+    <t>Bom Viver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quinta do Espinho, 5030-456 Santa Marta de Penaguiao, Vila Real </t>
+  </si>
+  <si>
+    <t>Calheiros Cruz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quinta de Covelos, Canelas, 5050 - 426 Peso da Regua, Vila Real </t>
+  </si>
+  <si>
+    <t>Caves Transmontanas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rua de Sao Domingos 22, 5070 Alijo, Vila Real </t>
+  </si>
+  <si>
+    <t>Caves Vale do Rodo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rua da Lousada, Peso da Regua 5050, Vila Real </t>
+  </si>
+  <si>
+    <t>D'Origem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rua da Praca 4, Loivos 5085-010, Vila Real </t>
+  </si>
+  <si>
+    <t>Folias de Baco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rua Antonio Candido 7, 5070-029 Alijo, Vila Real </t>
+  </si>
+  <si>
+    <t>Joao Brito e Cunha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rua Augusto Cesar 99, 5000-591 Vila Real </t>
+  </si>
+  <si>
+    <t>Lavradores de Feitoria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lote 5, Zona Industrial de Sabrosa, Sabrosa 5060, Vila Real </t>
+  </si>
+  <si>
+    <t>Manuel Hespanhol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vilarinho dos Freires, 5050-062 Peso da Regua, Vila Real </t>
+  </si>
+  <si>
+    <t>Paco de Teixeiro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quinta do Cotto Cidadelhe, 5040-154 Mesao Frio, Vila Real </t>
+  </si>
+  <si>
+    <t>Quinta Da Foz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gouvaes do Douro, 5085-243 Pinhao, Vila Real </t>
+  </si>
+  <si>
+    <t>Quinta da Pedra Alta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rua Direita 41, 5070-272 Alijo, Vila Real </t>
+  </si>
+  <si>
+    <t>Quinta da Romaneira</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cotas, Alijo 5070, Vila Real </t>
+  </si>
+  <si>
+    <t>Quinta da Vale Figueira</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quinta de Val da Figueira, 5085 - 220 Pinhao, Vila Real </t>
+  </si>
+  <si>
+    <t>Quinta de Boucos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Largo do Eiro, Sao Martinho de Anta 5060-433, Sao Martinho de Anta, Vila Real </t>
+  </si>
+  <si>
+    <t>Quinta de Santa Eugenia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Largo da Fonte, Santa Eugenia 5070, Vila Real </t>
+  </si>
+  <si>
+    <t>Quinta do Beato</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Torre, Poiares, 5050-345 Peso da Regua, Vila Real </t>
+  </si>
+  <si>
+    <t>Quinta do Bucheiro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rua de Sao Caetano, 5060-024 Sabrosa, Vila Real </t>
+  </si>
+  <si>
+    <t>Quinta do Passadouro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vale de Mendiz, Pinhao 5085, Alijo, Vila Real </t>
+  </si>
+  <si>
+    <t>Quinta do Vallado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vilarinho dos Freires, Peso da Regua 5050, Vila Real </t>
+  </si>
+  <si>
+    <t>Quinta Seara d'Ordens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Poiares 5050, Vila Real </t>
+  </si>
+  <si>
+    <t>Quinta Vale do Bragao</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quinta Vale do Bragao, 5060-033 Celeiros do Douro, Vila Real </t>
+  </si>
+  <si>
+    <t>Romarigo Vinhos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rua Dr Manuel de Arriaga, 5050-225 Peso da Regua, Vila Real </t>
+  </si>
+  <si>
+    <t>Tellu's</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rua da Lousada, 5050-262 Godim, Vila Real </t>
+  </si>
+  <si>
+    <t>Vinhas da Ciderma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rua Dr. Otilio Figueiredo, Quinta dos Barreiros, 5000-587 Vila Real </t>
   </si>
 </sst>
 </file>
@@ -437,24 +608,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95A0C55A-ED09-4DBE-BEFD-BE22C45A84AB}">
   <dimension ref="A1:B249"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD249"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="22.42578125" style="3"/>
+    <col min="1" max="1" width="22.42578125" style="3"/>
+    <col min="2" max="2" width="33.85546875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="19.5" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -462,7 +634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -470,7 +642,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -479,116 +651,228 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="2"/>
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="2"/>
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="2"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="2"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="2"/>
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="2"/>
+      <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="2"/>
+      <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="2"/>
+      <c r="A12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="2"/>
+      <c r="A13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="2"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="2"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="2"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="2"/>
+      <c r="A14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="2"/>
+      <c r="A18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="2"/>
+      <c r="A19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="2"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="2"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="2"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="2"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="2"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="2"/>
+      <c r="A20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="2"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="B27" s="2"/>
+      <c r="A26" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="B28" s="2"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="2"/>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="2"/>
+      <c r="A28" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="2"/>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-      <c r="B32" s="2"/>
+      <c r="A31" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
@@ -1459,12 +1743,7 @@
       <c r="B249" s="2"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://www.wine-searcher.com/merchant/26999" xr:uid="{1C57B3B3-511D-4377-B88E-E9CE1DA01797}"/>
-    <hyperlink ref="A3" r:id="rId2" display="https://www.wine-searcher.com/merchant/53939" xr:uid="{5877A6D1-BFF8-407C-BF90-0BB6A3EBA518}"/>
-    <hyperlink ref="A4" r:id="rId3" display="https://www.wine-searcher.com/merchant/95858" xr:uid="{BD73F3A3-6651-4F6F-9A21-B9D539CB4A85}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>